<commit_message>
Added weather data and python sunlight simulation model
</commit_message>
<xml_diff>
--- a/data/Main.xlsx
+++ b/data/Main.xlsx
@@ -5,18 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhe\Documents\MECH431\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moochster\OneDrive\Documents\2018 UBC\MECH 431\MECH431\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D398601-D5C5-4012-9FE8-251220782895}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="13_ncr:1_{3D398601-D5C5-4012-9FE8-251220782895}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{7E82490C-D8E3-419E-8188-6A44EBBFA76C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1350" windowWidth="28800" windowHeight="12360" activeTab="3" xr2:uid="{B79B3171-F36B-48DE-8068-476A01F57370}"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="28800" windowHeight="12360" activeTab="5" xr2:uid="{B79B3171-F36B-48DE-8068-476A01F57370}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="1" r:id="rId1"/>
     <sheet name="Parts" sheetId="3" r:id="rId2"/>
     <sheet name="Design Spec" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="4" r:id="rId4"/>
+    <sheet name="Analysis (Nothing)" sheetId="5" r:id="rId5"/>
+    <sheet name="Weather Data" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="76">
   <si>
     <t>Daily average demand</t>
   </si>
@@ -223,6 +225,39 @@
   </si>
   <si>
     <t>&lt;- eff in 2058</t>
+  </si>
+  <si>
+    <t>This is the analysis for doing nothing</t>
+  </si>
+  <si>
+    <t>Analysis period</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>Edmonton Weather Data</t>
+  </si>
+  <si>
+    <t>Longest Day</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>Sunrise</t>
+  </si>
+  <si>
+    <t>Shortest Day</t>
+  </si>
+  <si>
+    <t>Sun highest</t>
+  </si>
+  <si>
+    <t>deg</t>
+  </si>
+  <si>
+    <t>Sun lowest</t>
   </si>
 </sst>
 </file>
@@ -230,8 +265,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -276,23 +311,24 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -612,7 +648,7 @@
   <dimension ref="B2:P24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,25 +707,25 @@
       <c r="C7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6" t="s">
+      <c r="E7" s="8"/>
+      <c r="F7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6" t="s">
+      <c r="G7" s="8"/>
+      <c r="H7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6" t="s">
+      <c r="I7" s="8"/>
+      <c r="J7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K7" s="6"/>
+      <c r="K7" s="8"/>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
@@ -724,7 +760,7 @@
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
+      <c r="B9" s="7"/>
       <c r="C9" t="s">
         <v>6</v>
       </c>
@@ -760,7 +796,7 @@
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
+      <c r="B10" s="7"/>
       <c r="C10" t="s">
         <v>7</v>
       </c>
@@ -846,7 +882,7 @@
       </c>
     </row>
     <row r="15" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="D15" s="7"/>
+      <c r="D15" s="5"/>
       <c r="M15">
         <v>27</v>
       </c>
@@ -973,7 +1009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53B6EDC1-B39B-4E7B-8F88-7A2BF6E72A01}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
@@ -1088,13 +1124,13 @@
       <c r="B25" t="s">
         <v>62</v>
       </c>
-      <c r="J25" s="7">
+      <c r="J25" s="5">
         <v>0.35499999999999998</v>
       </c>
       <c r="K25" s="3">
         <v>0.32</v>
       </c>
-      <c r="L25" s="8">
+      <c r="L25" s="6">
         <f>(J25/K25)^(1/9)-1</f>
         <v>1.1599738260738901E-2</v>
       </c>
@@ -1106,7 +1142,7 @@
       <c r="J27">
         <v>2018</v>
       </c>
-      <c r="K27" s="7">
+      <c r="K27" s="5">
         <v>0.35499999999999998</v>
       </c>
     </row>
@@ -1117,7 +1153,7 @@
       <c r="J28">
         <v>2028</v>
       </c>
-      <c r="K28" s="8">
+      <c r="K28" s="6">
         <f>K27*(1+$L$25)^10</f>
         <v>0.39839642816971721</v>
       </c>
@@ -1126,7 +1162,7 @@
       <c r="J29">
         <v>2038</v>
       </c>
-      <c r="K29" s="8">
+      <c r="K29" s="6">
         <f t="shared" ref="K29:K31" si="0">K28*(1+$L$25)^10</f>
         <v>0.4470977858546159</v>
       </c>
@@ -1135,7 +1171,7 @@
       <c r="J30">
         <v>2048</v>
       </c>
-      <c r="K30" s="8">
+      <c r="K30" s="6">
         <f t="shared" si="0"/>
         <v>0.50175256599174112</v>
       </c>
@@ -1144,7 +1180,7 @@
       <c r="J31">
         <v>2058</v>
       </c>
-      <c r="K31" s="8">
+      <c r="K31" s="6">
         <f t="shared" si="0"/>
         <v>0.56308853553830984</v>
       </c>
@@ -1155,4 +1191,135 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66C03071-2F06-4341-ACA6-62B4A36D3BF8}">
+  <dimension ref="B2:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{385E2F3A-9060-42BF-ADCF-A98F8EA8DC7E}">
+  <dimension ref="A2:K8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0.21111111111111111</v>
+      </c>
+      <c r="I5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5">
+        <v>60</v>
+      </c>
+      <c r="K5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6">
+        <v>7.6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0.36805555555555558</v>
+      </c>
+      <c r="I6" t="s">
+        <v>75</v>
+      </c>
+      <c r="J6">
+        <v>13</v>
+      </c>
+      <c r="K6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>